<commit_message>
Polish project structure and logic
</commit_message>
<xml_diff>
--- a/settings/config.xlsx
+++ b/settings/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyrylo.Kondrashov\Documents\UiPath\git\Barfoot\settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyrylo.kondrashov\Documents\Barfoot_datascrapping-main\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D976E6-334B-4BF2-A172-46D149DDAF70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC36A2E-2D5B-402C-9B10-92E5B4F97772}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -361,13 +361,34 @@
   </si>
   <si>
     <t>unableToClickOnButtonGrLog</t>
+  </si>
+  <si>
+    <t>chromeClosed</t>
+  </si>
+  <si>
+    <t>Successfully close Google Chrome</t>
+  </si>
+  <si>
+    <t>chromeNotClosed</t>
+  </si>
+  <si>
+    <t>Unable to close Google Chrome</t>
+  </si>
+  <si>
+    <t>kyrylo.kondrashov@trinetix.com</t>
+  </si>
+  <si>
+    <t>emailNotSend</t>
+  </si>
+  <si>
+    <t>Email is not send successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -407,6 +428,12 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -425,10 +452,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -440,8 +468,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -756,16 +786,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="7" customFormat="1" ht="14.25" customHeight="1">
@@ -816,7 +846,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="14.5">
+    <row r="4" spans="1:26" ht="14.4">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
@@ -1002,7 +1032,9 @@
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
@@ -1987,8 +2019,11 @@
     <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1"/>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" xr:uid="{7763C804-5DDA-46A9-8402-6BC5B6EB9B57}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2000,10 +2035,10 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="27.81640625" customWidth="1"/>
-    <col min="2" max="2" width="59.36328125" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2245,18 +2280,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="60.26953125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.21875" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="14.25" customHeight="1">
@@ -2362,31 +2397,52 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -3353,6 +3409,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>